<commit_message>
Update BigML and WEKA jar
</commit_message>
<xml_diff>
--- a/File/Adult/Comparison.xlsx
+++ b/File/Adult/Comparison.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="2920" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
-    <sheet name="BigML vs OpusMiner" sheetId="2" r:id="rId2"/>
-    <sheet name="Apriori vs OpusMiner" sheetId="3" r:id="rId3"/>
+    <sheet name="BigML vs OpusMiner-BK" sheetId="2" r:id="rId2"/>
+    <sheet name="Apriori vs OpusMiner-BK" sheetId="3" r:id="rId3"/>
+    <sheet name="BigML vs OpusMiner-Layerd" sheetId="4" r:id="rId4"/>
+    <sheet name="BigML vs OpusMiner" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="129">
   <si>
     <t>Search by leverage</t>
   </si>
@@ -519,6 +521,52 @@
   </si>
   <si>
     <t>30/72</t>
+  </si>
+  <si>
+    <t>OpusMiner (p-value 0.05)</t>
+  </si>
+  <si>
+    <t>OpusMiner (p-value 0.05)2</t>
+  </si>
+  <si>
+    <t>Index: 30, field4 = EduNum13</t>
+  </si>
+  <si>
+    <t># of self-sufficent itemsets (out of 100) - After change on Independent Productivity</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Non</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-self-sufficent itemsets (out of 100) - After change on Independent Productivity</t>
+    </r>
+  </si>
+  <si>
+    <t>Index: 31, field3 = Bachelors</t>
+  </si>
+  <si>
+    <t>Layered: 13
+Non-layered: 13</t>
+  </si>
+  <si>
+    <t>Layered: 17
+Non-layered: 17</t>
   </si>
 </sst>
 </file>
@@ -703,12 +751,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -718,6 +763,15 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
@@ -865,14 +919,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G16" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A2:G16"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:I16" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A2:I16"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="Description" dataDxfId="8"/>
     <tableColumn id="2" name="OpusMiner (With layered critical values)" dataDxfId="7"/>
+    <tableColumn id="5" name="OpusMiner (p-value 0.05)" dataDxfId="1"/>
     <tableColumn id="3" name="BigML" dataDxfId="6"/>
     <tableColumn id="4" name="Apriori" dataDxfId="5"/>
     <tableColumn id="6" name="OpusMiner (With layered critical values)2" dataDxfId="4"/>
+    <tableColumn id="9" name="OpusMiner (p-value 0.05)2" dataDxfId="0"/>
     <tableColumn id="7" name="BigML2" dataDxfId="3"/>
     <tableColumn id="8" name="Apriori2" dataDxfId="2"/>
   </tableColumns>
@@ -1143,35 +1199,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" style="14" customWidth="1"/>
     <col min="2" max="2" width="33" style="14" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11" style="14"/>
+    <col min="3" max="3" width="22.1640625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="7.5" style="14" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" style="14" customWidth="1"/>
+    <col min="8" max="16384" width="11" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="15" t="s">
         <v>112</v>
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="15"/>
       <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>33</v>
       </c>
@@ -1179,53 +1239,99 @@
         <v>116</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>74</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="14">
         <v>36</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="F4" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="I4" s="14" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="14">
+        <v>32</v>
+      </c>
+      <c r="C5" s="14">
+        <v>18</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="14">
+        <v>66</v>
+      </c>
+      <c r="G5" s="14">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="14">
+        <v>68</v>
+      </c>
+      <c r="C6" s="14">
+        <v>82</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="14">
+        <v>34</v>
+      </c>
+      <c r="G6" s="14">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1238,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="107" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="107" workbookViewId="0">
       <selection activeCell="G11" sqref="G11:K11"/>
     </sheetView>
   </sheetViews>
@@ -1785,7 +1891,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView zoomScale="119" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G11" sqref="G11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2185,4 +2291,360 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>